<commit_message>
Can find n number of books in the Amazon book details file, as specified by the user.
My 1st Scrapping Project
</commit_message>
<xml_diff>
--- a/amazon_book_details.xlsx
+++ b/amazon_book_details.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,12 +458,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>The Time Machine</t>
+          <t>Dopamine Detox: A Short Guide to Remove Distractions and Get Your Brain to Do Hard Things</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>289.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -473,51 +473,95 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>H. G. Wells</t>
+          <t>Thibaut Meurisse</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>The Time Machine</t>
+          <t>Don't Believe Everything You Think (English)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>184.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4.4 out of 5 stars</t>
+          <t>4.5 out of 5 stars</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>H. G. Wells</t>
+          <t>Joseph Nguyen</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>The Time Machine</t>
+          <t>The Psychology of Money</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>160.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>4.6 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Morgan Housel</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>White Nights – Fyodor Dostoyevsky | A Million-Copy Bestseller | A Timeless Story of Love, Longing &amp; Solitude – Penguin Classics</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>89.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Fyodor Dostoyevsky</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>The Art of Being Alone: Loneliness Was My Cage, Solitude Is My Home (English)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>199.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>4.4 out of 5 stars</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>H. G. Wells</t>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Renuka Gavrani</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Can find n number of books in the Amazon book details file, as specified by the user. My 1st Scrapping Project
</commit_message>
<xml_diff>
--- a/amazon_book_details.xlsx
+++ b/amazon_book_details.xlsx
@@ -1,37 +1,114 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Backup\Web Scrapping\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2C051E-848F-4C8B-A540-F36E43A29EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Dopamine Detox: A Short Guide to Remove Distractions and Get Your Brain to Do Hard Things</t>
+  </si>
+  <si>
+    <t>289.</t>
+  </si>
+  <si>
+    <t>4.4 out of 5 stars</t>
+  </si>
+  <si>
+    <t>Thibaut Meurisse</t>
+  </si>
+  <si>
+    <t>Don't Believe Everything You Think (English)</t>
+  </si>
+  <si>
+    <t>184.</t>
+  </si>
+  <si>
+    <t>4.5 out of 5 stars</t>
+  </si>
+  <si>
+    <t>Joseph Nguyen</t>
+  </si>
+  <si>
+    <t>The Psychology of Money</t>
+  </si>
+  <si>
+    <t>160.</t>
+  </si>
+  <si>
+    <t>4.6 out of 5 stars</t>
+  </si>
+  <si>
+    <t>Morgan Housel</t>
+  </si>
+  <si>
+    <t>White Nights – Fyodor Dostoyevsky | A Million-Copy Bestseller | A Timeless Story of Love, Longing &amp; Solitude – Penguin Classics</t>
+  </si>
+  <si>
+    <t>89.</t>
+  </si>
+  <si>
+    <t>Fyodor Dostoyevsky</t>
+  </si>
+  <si>
+    <t>The Art of Being Alone: Loneliness Was My Cage, Solitude Is My Home (English)</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>Renuka Gavrani</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +123,52 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,149 +456,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.08984375" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="8.7265625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Rating</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Author</t>
-        </is>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Dopamine Detox: A Short Guide to Remove Distractions and Get Your Brain to Do Hard Things</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>289.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>4.4 out of 5 stars</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Thibaut Meurisse</t>
-        </is>
+    <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Don't Believe Everything You Think (English)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>184.</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>4.5 out of 5 stars</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Joseph Nguyen</t>
-        </is>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>The Psychology of Money</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>160.</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>4.6 out of 5 stars</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Morgan Housel</t>
-        </is>
+    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>White Nights – Fyodor Dostoyevsky | A Million-Copy Bestseller | A Timeless Story of Love, Longing &amp; Solitude – Penguin Classics</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>89.</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>4.6 out of 5 stars</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Fyodor Dostoyevsky</t>
-        </is>
+    <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>The Art of Being Alone: Loneliness Was My Cage, Solitude Is My Home (English)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>199.</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>4.4 out of 5 stars</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Renuka Gavrani</t>
-        </is>
+    <row r="6" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
my 1st venture into web scrapping with Python using BeautifulSoup.
</commit_message>
<xml_diff>
--- a/amazon_book_details.xlsx
+++ b/amazon_book_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Backup\Web Scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2C051E-848F-4C8B-A540-F36E43A29EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368ABB2E-F059-46E2-AAC2-FEE5F775D907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>Title</t>
   </si>
@@ -82,10 +82,106 @@
     <t>The Art of Being Alone: Loneliness Was My Cage, Solitude Is My Home (English)</t>
   </si>
   <si>
-    <t>184</t>
+    <t>199.</t>
   </si>
   <si>
     <t>Renuka Gavrani</t>
+  </si>
+  <si>
+    <t>Heart Lamp: Selected Stories | WINNER OF THE INTERNATIONAL BOOKER PRIZE 2025</t>
+  </si>
+  <si>
+    <t>622.</t>
+  </si>
+  <si>
+    <t>Dr Banu Mushtaq</t>
+  </si>
+  <si>
+    <t>Metamorphosis by Franz Kafka [Premium Paperback]: An Unsettling Exploration of Identity and Alienation | Existential Literature |Classic Literature| Psychological Fiction| Metaphorical Allegory</t>
+  </si>
+  <si>
+    <t>99.</t>
+  </si>
+  <si>
+    <t>Franz Kafka</t>
+  </si>
+  <si>
+    <t>Can We Be Strangers Again?: A moving tale of love, loyalty and the bittersweet beauty of letting go</t>
+  </si>
+  <si>
+    <t>197.</t>
+  </si>
+  <si>
+    <t>4.3 out of 5 stars</t>
+  </si>
+  <si>
+    <t>Shrijeet Shandilya</t>
+  </si>
+  <si>
+    <t>The Mountain Is You: Transforming Self-Sabotage Into Self-Mastery (English)</t>
+  </si>
+  <si>
+    <t>367.</t>
+  </si>
+  <si>
+    <t>Brianna Wiest</t>
+  </si>
+  <si>
+    <t>Read People Like a Book</t>
+  </si>
+  <si>
+    <t>399.</t>
+  </si>
+  <si>
+    <t>Patrick King</t>
+  </si>
+  <si>
+    <t>You Become What You Think: Master Your Mind, Master Your LIife</t>
+  </si>
+  <si>
+    <t>118.</t>
+  </si>
+  <si>
+    <t>Shubham Kumar Singh</t>
+  </si>
+  <si>
+    <t>The Alchemist</t>
+  </si>
+  <si>
+    <t>Paulo Coelho</t>
+  </si>
+  <si>
+    <t>World’s Greatest Books For Personal Growth &amp; Wealth (Set of 4 Books) : Perfect Motivational Gift Set</t>
+  </si>
+  <si>
+    <t>336.</t>
+  </si>
+  <si>
+    <t>Dale Carnegie</t>
+  </si>
+  <si>
+    <t>Days at the Morisaki Bookshop: The perfect book to curl up with - for lovers of Japanese translated fiction everywhere</t>
+  </si>
+  <si>
+    <t>272.</t>
+  </si>
+  <si>
+    <t>Satoshi Yagisawa</t>
+  </si>
+  <si>
+    <t>The Science of Self-Discipline: The Willpower, Mental Toughness and Self-Control to Resist Temptation and Achieve Your Goals</t>
+  </si>
+  <si>
+    <t>Peter Hollins</t>
+  </si>
+  <si>
+    <t>Rich Dad Poor Dad: What the Rich Teach Their Kids About Money That the Poor and Middle Class Do Not!</t>
+  </si>
+  <si>
+    <t>840.</t>
+  </si>
+  <si>
+    <t>Robert T. Kiyosaki</t>
   </si>
 </sst>
 </file>
@@ -141,19 +237,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,16 +544,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.08984375" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="39.453125" customWidth="1"/>
+    <col min="2" max="4" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -483,74 +570,228 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>